<commit_message>
initialize section content based identification
</commit_message>
<xml_diff>
--- a/headers.xlsx
+++ b/headers.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-3240" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="25600" yWindow="-3240" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
-    <sheet name="工作表4" sheetId="4" r:id="rId3"/>
-    <sheet name="工作表6" sheetId="6" r:id="rId4"/>
-    <sheet name="工作表5" sheetId="5" r:id="rId5"/>
-    <sheet name="工作表3" sheetId="3" r:id="rId6"/>
+    <sheet name="工作表7" sheetId="7" r:id="rId2"/>
+    <sheet name="工作表2" sheetId="2" r:id="rId3"/>
+    <sheet name="工作表4" sheetId="4" r:id="rId4"/>
+    <sheet name="工作表6" sheetId="6" r:id="rId5"/>
+    <sheet name="工作表5" sheetId="5" r:id="rId6"/>
+    <sheet name="工作表3" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7539" uniqueCount="1438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7606" uniqueCount="1441">
   <si>
     <t>Introduction</t>
   </si>
@@ -4364,6 +4365,18 @@
   </si>
   <si>
     <t>Petri nets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conclusion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4725,8 +4738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection sqref="A1:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4953,7 +4966,7 @@
         <v>2.3843181097452822E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>150</v>
+        <v>1438</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -5033,7 +5046,7 @@
         <v>1.691489876322904E-2</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>1438</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -5293,7 +5306,7 @@
         <v>7.8850195378636807E-3</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>1438</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
@@ -5352,6 +5365,9 @@
         <f t="shared" si="1"/>
         <v>7.2131535240716159E-3</v>
       </c>
+      <c r="E31" t="s">
+        <v>1284</v>
+      </c>
       <c r="F31">
         <f t="shared" si="0"/>
         <v>1342</v>
@@ -5369,6 +5385,9 @@
         <f t="shared" si="1"/>
         <v>7.2077785959612792E-3</v>
       </c>
+      <c r="E32" t="s">
+        <v>1284</v>
+      </c>
       <c r="F32">
         <f t="shared" si="0"/>
         <v>1341</v>
@@ -5387,7 +5406,7 @@
         <v>6.9444071185547889E-3</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>1438</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -5406,6 +5425,9 @@
         <f t="shared" si="1"/>
         <v>6.7670344909136837E-3</v>
       </c>
+      <c r="E34" t="s">
+        <v>1439</v>
+      </c>
       <c r="F34">
         <f t="shared" si="0"/>
         <v>1259</v>
@@ -5423,6 +5445,9 @@
         <f t="shared" si="1"/>
         <v>6.3961644513004642E-3</v>
       </c>
+      <c r="E35" t="s">
+        <v>1284</v>
+      </c>
       <c r="F35">
         <f t="shared" si="0"/>
         <v>1190</v>
@@ -5440,6 +5465,9 @@
         <f t="shared" si="1"/>
         <v>6.1327929738939739E-3</v>
       </c>
+      <c r="E36" t="s">
+        <v>1438</v>
+      </c>
       <c r="F36">
         <f t="shared" si="0"/>
         <v>1141</v>
@@ -5458,7 +5486,7 @@
         <v>5.8264220716047919E-3</v>
       </c>
       <c r="E37" t="s">
-        <v>150</v>
+        <v>1438</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
@@ -5498,7 +5526,7 @@
         <v>5.5576756660879658E-3</v>
       </c>
       <c r="E39" t="s">
-        <v>150</v>
+        <v>1438</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
@@ -6754,6 +6782,274 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -7145,7 +7441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1453"/>
   <sheetViews>
@@ -30266,11 +30562,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E920"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -45919,7 +46215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C205"/>
   <sheetViews>
@@ -48197,7 +48493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>